<commit_message>
added demand gap measures to the dashboard in data. I also included data issues spotted potentially in a text file.
</commit_message>
<xml_diff>
--- a/personal/alexei/data_insights_and_issues.xlsx
+++ b/personal/alexei/data_insights_and_issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notanai\Desktop\data_scrum\data-analytics-project\personal\alexei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778A9B32-31A0-4481-8E13-DC9A15AB917E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FAF07A-04BE-417C-AFBA-0157340F9F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{E2DF724E-566C-4F25-9CD6-30941DDF9C14}"/>
+    <workbookView xWindow="-25320" yWindow="1935" windowWidth="25440" windowHeight="15270" xr2:uid="{E2DF724E-566C-4F25-9CD6-30941DDF9C14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>High-Level Insights we can already extract from the four datasets</t>
   </si>
@@ -513,54 +513,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (household size, device OS, join-date).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Confirmation that </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Title_1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is redundant; permission to drop duplicates.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Expected refresh frequency for the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Combined_information</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> file.</t>
     </r>
   </si>
 </sst>
@@ -762,50 +714,50 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,7 +766,7 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -829,23 +781,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -865,24 +801,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -902,26 +820,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -941,54 +839,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1027,6 +896,24 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1046,44 +933,26 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1103,6 +972,89 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1118,25 +1070,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9AAC5089-8B3D-4C53-97BA-694ADEDD6FBB}" name="Table3" displayName="Table3" ref="F7:H15" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9AAC5089-8B3D-4C53-97BA-694ADEDD6FBB}" name="Table3" displayName="Table3" ref="F7:H15" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="F7:H15" xr:uid="{9AAC5089-8B3D-4C53-97BA-694ADEDD6FBB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE668C7F-755B-43F2-89AC-EF92AC5A30EB}" name="Theme" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8B58AFC5-D848-4869-A167-2573979F06CD}" name="What the data currently shows" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8A85258D-0DC5-46BA-B8A4-6F3B058FCB3D}" name="Why it matters to StreamFlix" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{EE668C7F-755B-43F2-89AC-EF92AC5A30EB}" name="Theme" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{8B58AFC5-D848-4869-A167-2573979F06CD}" name="What the data currently shows" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{8A85258D-0DC5-46BA-B8A4-6F3B058FCB3D}" name="Why it matters to StreamFlix" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{62218E17-2969-4609-B464-681EB8C8AF87}" name="Table5" displayName="Table5" ref="F19:I26" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{62218E17-2969-4609-B464-681EB8C8AF87}" name="Table5" displayName="Table5" ref="F19:I26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="F19:I26" xr:uid="{62218E17-2969-4609-B464-681EB8C8AF87}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E2B4D900-3A77-464A-B94C-59B681B2F744}" name="Area" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{1E71378D-24E6-414A-9943-3CFAAEEC68AC}" name="Issue" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{3625F260-C9E4-4335-A93E-5B5D9511F443}" name="Impact" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{B326D455-CAD4-43ED-B228-FADF14683414}" name="Suggested fix" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E2B4D900-3A77-464A-B94C-59B681B2F744}" name="Area" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1E71378D-24E6-414A-9943-3CFAAEEC68AC}" name="Issue" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{3625F260-C9E4-4335-A93E-5B5D9511F443}" name="Impact" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B326D455-CAD4-43ED-B228-FADF14683414}" name="Suggested fix" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1441,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96953F1-41BA-47D2-8B79-89D0B626FF62}">
   <dimension ref="D6:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:D58"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,104 +1406,104 @@
   </cols>
   <sheetData>
     <row r="6" spans="6:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="6:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="6:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="6:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="6:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="6:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="6:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="6:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="6:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="6:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1684,64 +1636,64 @@
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="19"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="19"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="19"/>
+      <c r="D40" s="18"/>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="19" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="19"/>
+      <c r="D43" s="18"/>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="20" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1751,41 +1703,37 @@
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="19"/>
+      <c r="D51" s="18"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="22" t="s">
+      <c r="D52" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="19"/>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="19"/>
+      <c r="D55" s="18"/>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="22" t="s">
-        <v>74</v>
-      </c>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="6"/>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="6" t="s">
-        <v>75</v>
-      </c>
+      <c r="D58" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>